<commit_message>
Billing cash input. SpotStockTest print
</commit_message>
<xml_diff>
--- a/bin/print/ori/BillingReport.xlsx
+++ b/bin/print/ori/BillingReport.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Daily_Report1" localSheetId="0">Sheet1!$A$1:$M$72</definedName>
+    <definedName name="Daily_Report1" localSheetId="0">Sheet1!$A$1:$M$66</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -773,10 +773,44 @@
       <c r="C64" s="5"/>
     </row>
     <row r="65" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C65" s="5"/>
+      <c r="C65" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="4">
+        <v>232710.53</v>
+      </c>
+      <c r="E65" s="7">
+        <v>3008.49</v>
+      </c>
+      <c r="F65" s="7">
+        <v>0</v>
+      </c>
+      <c r="G65" s="7">
+        <v>10250.99</v>
+      </c>
+      <c r="H65" s="7">
+        <v>36935</v>
+      </c>
+      <c r="I65" s="7">
+        <v>0</v>
+      </c>
+      <c r="J65" s="7">
+        <v>0</v>
+      </c>
+      <c r="K65" s="7">
+        <v>180</v>
+      </c>
+      <c r="L65" s="7">
+        <v>472</v>
+      </c>
     </row>
     <row r="66" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C66" s="5"/>
+      <c r="C66" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D66" s="4">
+        <v>242961.52</v>
+      </c>
     </row>
     <row r="67" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C67" s="5"/>
@@ -791,44 +825,10 @@
       <c r="C70" s="5"/>
     </row>
     <row r="71" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C71" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D71" s="4">
-        <v>182625.8</v>
-      </c>
-      <c r="E71" s="7">
-        <v>2583.63</v>
-      </c>
-      <c r="F71" s="7">
-        <v>0</v>
-      </c>
-      <c r="G71" s="7">
-        <v>3304.37</v>
-      </c>
-      <c r="H71" s="7">
-        <v>32692</v>
-      </c>
-      <c r="I71" s="7">
-        <v>0</v>
-      </c>
-      <c r="J71" s="7">
-        <v>0</v>
-      </c>
-      <c r="K71" s="7">
-        <v>252</v>
-      </c>
-      <c r="L71" s="7">
-        <v>0</v>
-      </c>
+      <c r="C71" s="5"/>
     </row>
     <row r="72" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C72" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D72" s="4">
-        <v>185930.17</v>
-      </c>
+      <c r="C72" s="5"/>
     </row>
     <row r="73" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C73" s="5"/>

</xml_diff>